<commit_message>
cleaned optimization file, added lp file
</commit_message>
<xml_diff>
--- a/Assign_1/Problem_1/optimizationOutput.xlsx
+++ b/Assign_1/Problem_1/optimizationOutput.xlsx
@@ -2656,7 +2656,7 @@
         <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -2679,10 +2679,8 @@
       <c r="L2" t="n">
         <v>3</v>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="M2" t="n">
+        <v>11</v>
       </c>
       <c r="N2" t="n">
         <v>30</v>
@@ -3114,7 +3112,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -3165,7 +3163,7 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="N7" t="n">
         <v>17</v>
@@ -3689,8 +3687,10 @@
           <t>EDDT</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>11</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -3711,7 +3711,7 @@
         <v>109</v>
       </c>
       <c r="G13" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>

</xml_diff>